<commit_message>
Update to Clean ATDD sheet for chapter 9
</commit_message>
<xml_diff>
--- a/Excel sheets/Examples/Clean ATDD sheet.xlsx
+++ b/Excel sheets/Examples/Clean ATDD sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvvugt\source\repos\Automated-Testing-in-Microsoft-Dynamics-365-Business-Central-Second-Edition\ATDD Scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvvugt\source\repos\Automated-Testing-in-Microsoft-Dynamics-365-Business-Central-Second-Edition\Excel sheets\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE4FA88-D98D-41FF-B149-4C5435FAD60C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813B0455-1287-455A-B93A-E93A1EC2145A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{DB99ADC0-1D36-4CB0-890F-ABAEDD9356F9}"/>
+    <workbookView xWindow="2400" yWindow="3420" windowWidth="22290" windowHeight="8145" xr2:uid="{DB99ADC0-1D36-4CB0-890F-ABAEDD9356F9}"/>
   </bookViews>
   <sheets>
     <sheet name="ATDD Scenarios" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="45">
   <si>
     <t>Feature</t>
   </si>
@@ -76,9 +76,6 @@
     <t>Check that label can be assigned to customer</t>
   </si>
   <si>
-    <t>To make verification meaningful a customer record is created</t>
-  </si>
-  <si>
     <t>Given</t>
   </si>
   <si>
@@ -143,6 +140,36 @@
   </si>
   <si>
     <t>FEATURE</t>
+  </si>
+  <si>
+    <t>SubFeature</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>A positive-negative scenario</t>
+  </si>
+  <si>
+    <t>A UI scenario</t>
+  </si>
+  <si>
+    <t>A scenario</t>
   </si>
 </sst>
 </file>
@@ -296,85 +323,23 @@
   <dxfs count="30">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0070C0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0070C0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -440,26 +405,47 @@
       <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
-        <b val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
         <color rgb="FF00B050"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -501,6 +487,47 @@
     <dxf>
       <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -515,54 +542,54 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D77B0683-CDBE-450E-913A-81EFBBA8B17E}" name="Table2" displayName="Table2" ref="A1:L6" totalsRowShown="0" headerRowDxfId="29">
-  <autoFilter ref="A1:L6" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D77B0683-CDBE-450E-913A-81EFBBA8B17E}" name="Table2" displayName="Table2" ref="A1:L14" totalsRowShown="0" headerRowDxfId="24">
+  <autoFilter ref="A1:L14" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{8363E7FF-10AC-4A2B-AF58-2B6F4A3A2982}" name="Feature"/>
     <tableColumn id="9" xr3:uid="{47ED26B9-CBC1-4AA1-A3A9-843BF13AA89B}" name="Sub Feature"/>
-    <tableColumn id="10" xr3:uid="{2CFDA2E7-B629-4ECF-BE79-854343648AF6}" name="UI" dataDxfId="28"/>
-    <tableColumn id="12" xr3:uid="{42186982-BEE2-4B88-B732-989CDBD8F258}" name="Positive-negative" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{CF058E75-EBE8-492F-899F-08E1336AACB4}" name="Scenario" dataDxfId="26"/>
+    <tableColumn id="10" xr3:uid="{2CFDA2E7-B629-4ECF-BE79-854343648AF6}" name="UI" dataDxfId="23"/>
+    <tableColumn id="12" xr3:uid="{42186982-BEE2-4B88-B732-989CDBD8F258}" name="Positive-negative" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{CF058E75-EBE8-492F-899F-08E1336AACB4}" name="Scenario" dataDxfId="21"/>
     <tableColumn id="3" xr3:uid="{824F4994-529B-42E7-960A-C52362C8177D}" name="Given-When-Then (Tag)"/>
-    <tableColumn id="5" xr3:uid="{9A2C2A27-BDEF-4BD0-8B83-E6DCBCFA35E2}" name="Given-When-Then (Description)" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{357E2CE4-1423-477D-9378-4140E6CC741F}" name="Scenario #" dataDxfId="24"/>
-    <tableColumn id="6" xr3:uid="{A0EF38BD-226F-4389-8485-98738BF5C0B4}" name="ATDD Format" dataDxfId="23">
+    <tableColumn id="5" xr3:uid="{9A2C2A27-BDEF-4BD0-8B83-E6DCBCFA35E2}" name="Given-When-Then (Description)" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{357E2CE4-1423-477D-9378-4140E6CC741F}" name="Scenario #" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{A0EF38BD-226F-4389-8485-98738BF5C0B4}" name="ATDD Format" dataDxfId="18">
       <calculatedColumnFormula>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{55990E10-8959-4AC5-A765-C7364ECDCDE5}" name="Code Format" dataDxfId="22">
+    <tableColumn id="7" xr3:uid="{55990E10-8959-4AC5-A765-C7364ECDCDE5}" name="Code Format" dataDxfId="17">
       <calculatedColumnFormula>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{428C58FA-6B63-4AB1-8578-57C5373BC837}" name="ATDD.TestScriptor Format" dataDxfId="21">
-      <calculatedColumnFormula>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</calculatedColumnFormula>
+    <tableColumn id="11" xr3:uid="{428C58FA-6B63-4AB1-8578-57C5373BC837}" name="ATDD.TestScriptor Format" dataDxfId="0">
+      <calculatedColumnFormula>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{67272D7F-D0CB-4C6B-967E-B47CC34979CB}" name="Notes" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{67272D7F-D0CB-4C6B-967E-B47CC34979CB}" name="Notes" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AC94DC61-3A21-44B1-A4FA-D3AE0A291830}" name="Table23" displayName="Table23" ref="A1:L17" totalsRowShown="0" headerRowDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AC94DC61-3A21-44B1-A4FA-D3AE0A291830}" name="Table23" displayName="Table23" ref="A1:L17" totalsRowShown="0" headerRowDxfId="10">
   <autoFilter ref="A1:L17" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{EB12FABE-99EE-4C64-9371-664DA2BC018B}" name="Feature"/>
     <tableColumn id="9" xr3:uid="{C4BF811B-A50B-4F15-ABFB-76F5EF61BAEC}" name="Sub Feature"/>
-    <tableColumn id="10" xr3:uid="{050332A6-04F7-4C80-8BF0-1A37BF66834D}" name="UI" dataDxfId="18"/>
-    <tableColumn id="12" xr3:uid="{91F463C5-D5E2-4E74-89F7-26421CFD4688}" name="Positive-negative" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{F4B03F80-242C-48F3-AD45-4F8870F7CF4C}" name="Scenario" dataDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{050332A6-04F7-4C80-8BF0-1A37BF66834D}" name="UI" dataDxfId="9"/>
+    <tableColumn id="12" xr3:uid="{91F463C5-D5E2-4E74-89F7-26421CFD4688}" name="Positive-negative" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{F4B03F80-242C-48F3-AD45-4F8870F7CF4C}" name="Scenario" dataDxfId="7"/>
     <tableColumn id="3" xr3:uid="{CC6D9ED1-342A-442A-A781-19E1B48EC192}" name="Given-When-Then (Tag)"/>
-    <tableColumn id="5" xr3:uid="{4B77C75B-29B6-4D6D-8295-8BCB00B5A021}" name="Given-When-Then (Description)" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{7A8CEFC7-AFDE-40F5-BF03-D453506926E6}" name="Scenario #" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{4C548BB4-BEA7-4564-81EF-9BD6BCF666EF}" name="ATDD Format" dataDxfId="13">
+    <tableColumn id="5" xr3:uid="{4B77C75B-29B6-4D6D-8295-8BCB00B5A021}" name="Given-When-Then (Description)" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{7A8CEFC7-AFDE-40F5-BF03-D453506926E6}" name="Scenario #" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{4C548BB4-BEA7-4564-81EF-9BD6BCF666EF}" name="ATDD Format" dataDxfId="4">
       <calculatedColumnFormula>IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table23[[#This Row],[Scenario '#]],"0000"),"] ",Table23[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table23[[#This Row],[Given-When-Then (Tag)]]),"] ",Table23[[#This Row],[Given-When-Then (Description)]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{762A89F1-1CE0-4623-9ECE-7E18ABCC76DC}" name="Code Format" dataDxfId="12">
+    <tableColumn id="7" xr3:uid="{762A89F1-1CE0-4623-9ECE-7E18ABCC76DC}" name="Code Format" dataDxfId="3">
       <calculatedColumnFormula>_xlfn.CONCAT("//",Table23[[#This Row],[ATDD Format]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{01376FDB-C35B-4080-A02C-72B0C39BDC01}" name="ATDD.TestScriptor Format" dataDxfId="11">
+    <tableColumn id="11" xr3:uid="{01376FDB-C35B-4080-A02C-72B0C39BDC01}" name="ATDD.TestScriptor Format" dataDxfId="2">
       <calculatedColumnFormula>IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{108458B0-953E-40C3-A10B-F57A3E16C1B8}" name="Notes" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{108458B0-953E-40C3-A10B-F57A3E16C1B8}" name="Notes" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -865,10 +892,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08B1ED69-5F96-4A81-993F-0E906F475813}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -879,11 +906,9 @@
     <col min="4" max="4" width="9.5703125" style="5" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" style="6" customWidth="1"/>
     <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" style="7" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" style="7" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.140625" style="7" customWidth="1"/>
+    <col min="9" max="11" width="32.5703125" style="7" customWidth="1"/>
     <col min="12" max="12" width="8.5703125" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -898,7 +923,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -919,7 +944,7 @@
         <v>8</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>9</v>
@@ -929,26 +954,28 @@
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9"/>
+      <c r="B2" s="9" t="s">
+        <v>35</v>
+      </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
       <c r="E2" s="19"/>
       <c r="F2" s="11"/>
       <c r="G2" s="21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H2" s="12"/>
       <c r="I2" s="11" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v xml:space="preserve">[FEATURE] Feature </v>
+        <v>[FEATURE] Feature SubFeature</v>
       </c>
       <c r="J2" s="11" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v xml:space="preserve">//[FEATURE] Feature </v>
+        <v>//[FEATURE] Feature SubFeature</v>
       </c>
       <c r="K2" s="18" t="str">
-        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Feature 'Feature' {</v>
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Feature 'Feature SubFeature' {</v>
       </c>
       <c r="L2" s="11"/>
     </row>
@@ -956,34 +983,40 @@
       <c r="A3" t="s">
         <v>0</v>
       </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
       <c r="E3" s="6" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="H3" s="8">
         <v>1</v>
       </c>
       <c r="I3" s="15" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0001] Scenario</v>
+        <v>[SCENARIO #0001] A scenario</v>
       </c>
       <c r="J3" s="16" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0001] Scenario</v>
+        <v>//[SCENARIO #0001] A scenario</v>
       </c>
       <c r="K3" s="17" t="str">
-        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0001 'Scenario' {</v>
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0001 'A scenario' {</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H4" s="8">
         <v>1</v>
@@ -997,7 +1030,7 @@
         <v>//[GIVEN] A</v>
       </c>
       <c r="K4" s="17" t="str">
-        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Given 'A'</v>
       </c>
     </row>
@@ -1005,11 +1038,14 @@
       <c r="A5" t="s">
         <v>0</v>
       </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H5" s="8">
         <v>1</v>
@@ -1023,7 +1059,7 @@
         <v>//[WHEN] B</v>
       </c>
       <c r="K5" s="17" t="str">
-        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>When 'B'</v>
       </c>
     </row>
@@ -1031,11 +1067,14 @@
       <c r="A6" t="s">
         <v>0</v>
       </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H6" s="8">
         <v>1</v>
@@ -1049,13 +1088,263 @@
         <v>//[THEN] C</v>
       </c>
       <c r="K6" s="17" t="str">
-        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'C' } }</v>
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'C' }</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="8">
+        <v>2</v>
+      </c>
+      <c r="I7" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0002] A positive-negative scenario</v>
+      </c>
+      <c r="J7" s="16" t="str">
+        <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0002] A positive-negative scenario</v>
+      </c>
+      <c r="K7" s="16" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0002 'A positive-negative scenario' {</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="8">
+        <v>2</v>
+      </c>
+      <c r="I8" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] D</v>
+      </c>
+      <c r="J8" s="16" t="str">
+        <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] D</v>
+      </c>
+      <c r="K8" s="16" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'D'</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" s="8">
+        <v>2</v>
+      </c>
+      <c r="I9" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] E</v>
+      </c>
+      <c r="J9" s="16" t="str">
+        <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] E</v>
+      </c>
+      <c r="K9" s="16" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'E'</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" s="8">
+        <v>2</v>
+      </c>
+      <c r="I10" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] F</v>
+      </c>
+      <c r="J10" s="16" t="str">
+        <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] F</v>
+      </c>
+      <c r="K10" s="16" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'F' }</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" s="8">
+        <v>3</v>
+      </c>
+      <c r="I11" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0003] A UI scenario</v>
+      </c>
+      <c r="J11" s="16" t="str">
+        <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0003] A UI scenario</v>
+      </c>
+      <c r="K11" s="16" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0003 'A UI scenario' {</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H12" s="8">
+        <v>3</v>
+      </c>
+      <c r="I12" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] G</v>
+      </c>
+      <c r="J12" s="16" t="str">
+        <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] G</v>
+      </c>
+      <c r="K12" s="16" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'G'</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" s="8">
+        <v>3</v>
+      </c>
+      <c r="I13" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] H</v>
+      </c>
+      <c r="J13" s="16" t="str">
+        <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] H</v>
+      </c>
+      <c r="K13" s="16" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'H'</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" s="8">
+        <v>3</v>
+      </c>
+      <c r="I14" s="15" t="str">
+        <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] I</v>
+      </c>
+      <c r="J14" s="16" t="str">
+        <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] I</v>
+      </c>
+      <c r="K14" s="16" t="str">
+        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'I' } }</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:D1048576">
-    <cfRule type="cellIs" dxfId="9" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="13" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1072,18 +1361,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="3" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="4" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1099,22 +1388,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B9C69E6-B7EF-4C82-A3EA-E6EE3FD2884C}">
   <dimension ref="A1:L108"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" style="5" customWidth="1"/>
     <col min="4" max="4" width="9" style="5" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="6" customWidth="1"/>
     <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" style="8" customWidth="1"/>
-    <col min="9" max="11" width="46.140625" style="7" customWidth="1"/>
-    <col min="12" max="12" width="47.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="61.42578125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" style="8" customWidth="1"/>
+    <col min="9" max="11" width="43.42578125" style="7" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1128,7 +1417,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -1149,7 +1438,7 @@
         <v>8</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>9</v>
@@ -1167,7 +1456,7 @@
       <c r="E2" s="19"/>
       <c r="F2" s="9"/>
       <c r="G2" s="21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H2" s="12"/>
       <c r="I2" s="11" t="str">
@@ -1209,9 +1498,6 @@
         <f ca="1">IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0001 'Check that label can be assigned to customer' {</v>
       </c>
-      <c r="L3" s="7" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1221,10 +1507,10 @@
         <v>11</v>
       </c>
       <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>15</v>
       </c>
       <c r="H4" s="8">
         <v>1</v>
@@ -1250,10 +1536,10 @@
         <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H5" s="8">
         <v>1</v>
@@ -1279,10 +1565,10 @@
         <v>11</v>
       </c>
       <c r="F6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>17</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>18</v>
       </c>
       <c r="H6" s="8">
         <v>1</v>
@@ -1308,10 +1594,10 @@
         <v>11</v>
       </c>
       <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>20</v>
       </c>
       <c r="H7" s="8">
         <v>1</v>
@@ -1336,8 +1622,11 @@
       <c r="B8" t="s">
         <v>11</v>
       </c>
+      <c r="D8" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="E8" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H8" s="8">
         <v>2</v>
@@ -1362,11 +1651,14 @@
       <c r="B9" t="s">
         <v>11</v>
       </c>
+      <c r="D9" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="F9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H9" s="8">
         <v>2</v>
@@ -1391,11 +1683,14 @@
       <c r="B10" t="s">
         <v>11</v>
       </c>
+      <c r="D10" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="F10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H10" s="8">
         <v>2</v>
@@ -1420,11 +1715,14 @@
       <c r="B11" t="s">
         <v>11</v>
       </c>
+      <c r="D11" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="F11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H11" s="8">
         <v>2</v>
@@ -1449,11 +1747,14 @@
       <c r="B12" t="s">
         <v>11</v>
       </c>
+      <c r="D12" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="F12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H12" s="8">
         <v>2</v>
@@ -1479,10 +1780,10 @@
         <v>11</v>
       </c>
       <c r="C13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="H13" s="8">
         <v>3</v>
@@ -1508,13 +1809,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>15</v>
       </c>
       <c r="H14" s="8">
         <v>3</v>
@@ -1540,13 +1841,13 @@
         <v>11</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H15" s="8">
         <v>3</v>
@@ -1572,13 +1873,13 @@
         <v>11</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H16" s="8">
         <v>3</v>
@@ -1604,13 +1905,13 @@
         <v>11</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>20</v>
       </c>
       <c r="H17" s="8">
         <v>3</v>
@@ -1632,7 +1933,7 @@
     <row r="108" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="4" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1649,18 +1950,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fixed reference error in Clean ATDD sheet.xlsx
</commit_message>
<xml_diff>
--- a/Excel sheets/Examples/Clean ATDD sheet.xlsx
+++ b/Excel sheets/Examples/Clean ATDD sheet.xlsx
@@ -1,24 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvvugt\source\repos\Automated-Testing-in-Microsoft-Dynamics-365-Business-Central-Second-Edition\Excel sheets\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB94C7F-5AC2-4DCD-ADD4-E04251366A0A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61BA358C-B570-4F9F-B866-EDB5F5D3762F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="255" windowWidth="24510" windowHeight="15990" xr2:uid="{DB99ADC0-1D36-4CB0-890F-ABAEDD9356F9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{DB99ADC0-1D36-4CB0-890F-ABAEDD9356F9}"/>
   </bookViews>
   <sheets>
     <sheet name="ATDD Scenarios" sheetId="1" r:id="rId1"/>
     <sheet name="Examples" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -544,19 +541,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="ATDD Scenarios"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D77B0683-CDBE-450E-913A-81EFBBA8B17E}" name="Table2" displayName="Table2" ref="A1:L14" totalsRowShown="0" headerRowDxfId="24">
   <autoFilter ref="A1:L14" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
@@ -603,7 +587,7 @@
       <calculatedColumnFormula>_xlfn.CONCAT("//",Table23[[#This Row],[ATDD Format]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="11" xr3:uid="{01376FDB-C35B-4080-A02C-72B0C39BDC01}" name="ATDD.TestScriptor Format" dataDxfId="0">
-      <calculatedColumnFormula>[1]!Table29[[#This Row],[ATDD.TestScriptor Format]]</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{108458B0-953E-40C3-A10B-F57A3E16C1B8}" name="Notes" dataDxfId="1"/>
   </tableColumns>
@@ -911,7 +895,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1108,7 +1092,7 @@
         <v>Then 'C' }</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1132,7 +1116,7 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[SCENARIO #0002] A positive-negative scenario</v>
       </c>
-      <c r="K7" s="16" t="str">
+      <c r="K7" s="17" t="str">
         <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0002 'A positive-negative scenario' {</v>
       </c>
@@ -1164,7 +1148,7 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] D</v>
       </c>
-      <c r="K8" s="16" t="str">
+      <c r="K8" s="17" t="str">
         <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Given 'D'</v>
       </c>
@@ -1196,7 +1180,7 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[WHEN] E</v>
       </c>
-      <c r="K9" s="16" t="str">
+      <c r="K9" s="17" t="str">
         <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>When 'E'</v>
       </c>
@@ -1228,12 +1212,12 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[THEN] F</v>
       </c>
-      <c r="K10" s="16" t="str">
+      <c r="K10" s="17" t="str">
         <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Then 'F' }</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1257,7 +1241,7 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[SCENARIO #0003] A UI scenario</v>
       </c>
-      <c r="K11" s="16" t="str">
+      <c r="K11" s="17" t="str">
         <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0003 'A UI scenario' {</v>
       </c>
@@ -1289,7 +1273,7 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] G</v>
       </c>
-      <c r="K12" s="16" t="str">
+      <c r="K12" s="17" t="str">
         <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Given 'G'</v>
       </c>
@@ -1321,7 +1305,7 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[WHEN] H</v>
       </c>
-      <c r="K13" s="16" t="str">
+      <c r="K13" s="17" t="str">
         <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>When 'H'</v>
       </c>
@@ -1353,7 +1337,7 @@
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v>//[THEN] I</v>
       </c>
-      <c r="K14" s="16" t="str">
+      <c r="K14" s="17" t="str">
         <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Then 'I' } }</v>
       </c>
@@ -1405,7 +1389,7 @@
   <dimension ref="A1:L108"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1484,8 +1468,8 @@
         <v>//[FEATURE] Label UT Customer</v>
       </c>
       <c r="K2" s="18" t="str">
-        <f ca="1">[1]!Table29[[#This Row],[ATDD.TestScriptor Format]]</f>
-        <v>Feature 'LookupValue UT Customer' {</v>
+        <f ca="1">IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Feature 'Label UT Customer' {</v>
       </c>
       <c r="L2" s="11"/>
     </row>
@@ -1511,8 +1495,8 @@
         <v>//[SCENARIO #0001] Check that label can be assigned to customer</v>
       </c>
       <c r="K3" s="17" t="str">
-        <f ca="1">[1]!Table29[[#This Row],[ATDD.TestScriptor Format]]</f>
-        <v>Scenario 0001 'Assign lookup value to customer' {</v>
+        <f ca="1">IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0001 'Check that label can be assigned to customer' {</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1540,8 +1524,8 @@
         <v>//[GIVEN] A label</v>
       </c>
       <c r="K4" s="17" t="str">
-        <f ca="1">[1]!Table29[[#This Row],[ATDD.TestScriptor Format]]</f>
-        <v>Given 'Lookup value'</v>
+        <f ca="1">IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'A label'</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1569,8 +1553,8 @@
         <v>//[GIVEN] A customer</v>
       </c>
       <c r="K5" s="17" t="str">
-        <f ca="1">[1]!Table29[[#This Row],[ATDD.TestScriptor Format]]</f>
-        <v>Given 'Customer'</v>
+        <f ca="1">IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'A customer'</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1598,8 +1582,8 @@
         <v>//[WHEN] Assign label to customer</v>
       </c>
       <c r="K6" s="17" t="str">
-        <f ca="1">[1]!Table29[[#This Row],[ATDD.TestScriptor Format]]</f>
-        <v>When 'Set lookup value on customer'</v>
+        <f ca="1">IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Assign label to customer'</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="26.25" x14ac:dyDescent="0.25">
@@ -1627,8 +1611,8 @@
         <v>//[THEN] Customer has label field populated</v>
       </c>
       <c r="K7" s="17" t="str">
-        <f ca="1">[1]!Table29[[#This Row],[ATDD.TestScriptor Format]]</f>
-        <v>Then 'Customer has lookup value code field populated' }</v>
+        <f ca="1">IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Customer has label field populated' }</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -1656,8 +1640,8 @@
         <v>//[SCENARIO #0002] Check that label field table relation is validated for non-existing label on customer</v>
       </c>
       <c r="K8" s="17" t="str">
-        <f ca="1">[1]!Table29[[#This Row],[ATDD.TestScriptor Format]]</f>
-        <v>Scenario 0002 'Assign non-existing lookup value to customer' {</v>
+        <f ca="1">IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0002 'Check that label field table relation is validated for non-existing label on customer' {</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1688,8 +1672,8 @@
         <v>//[GIVEN] A non-existing label value</v>
       </c>
       <c r="K9" s="17" t="str">
-        <f ca="1">[1]!Table29[[#This Row],[ATDD.TestScriptor Format]]</f>
-        <v>Given 'Non-existing lookup value'</v>
+        <f ca="1">IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'A non-existing label value'</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1720,8 +1704,8 @@
         <v>//[GIVEN] A customer record variable</v>
       </c>
       <c r="K10" s="17" t="str">
-        <f ca="1">[1]!Table29[[#This Row],[ATDD.TestScriptor Format]]</f>
-        <v>Given 'Customer record variable'</v>
+        <f ca="1">IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'A customer record variable'</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1752,8 +1736,8 @@
         <v>//[WHEN] Assign non-existing label to customer</v>
       </c>
       <c r="K11" s="17" t="str">
-        <f ca="1">[1]!Table29[[#This Row],[ATDD.TestScriptor Format]]</f>
-        <v>When 'Set non-existing lookup value on customer'</v>
+        <f ca="1">IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Assign non-existing label to customer'</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="26.25" x14ac:dyDescent="0.25">
@@ -1784,8 +1768,8 @@
         <v>//[THEN] Non existing label error was thrown</v>
       </c>
       <c r="K12" s="17" t="str">
-        <f ca="1">[1]!Table29[[#This Row],[ATDD.TestScriptor Format]]</f>
-        <v>Then 'Non existing lookup value error thrown' }</v>
+        <f ca="1">IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Non existing label error was thrown' }</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -1813,8 +1797,8 @@
         <v>//[SCENARIO #0003] Check that label can be assigned on customer card</v>
       </c>
       <c r="K13" s="17" t="str">
-        <f ca="1">[1]!Table29[[#This Row],[ATDD.TestScriptor Format]]</f>
-        <v>Scenario 0003 'Assign lookup value on customer card' {</v>
+        <f ca="1">IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0003 'Check that label can be assigned on customer card' {</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1845,8 +1829,8 @@
         <v>//[GIVEN] A label</v>
       </c>
       <c r="K14" s="17" t="str">
-        <f ca="1">[1]!Table29[[#This Row],[ATDD.TestScriptor Format]]</f>
-        <v>Given 'Lookup value'</v>
+        <f ca="1">IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'A label'</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1877,8 +1861,8 @@
         <v>//[GIVEN] A customer card</v>
       </c>
       <c r="K15" s="17" t="str">
-        <f ca="1">[1]!Table29[[#This Row],[ATDD.TestScriptor Format]]</f>
-        <v>Given 'Customer card'</v>
+        <f ca="1">IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'A customer card'</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1909,8 +1893,8 @@
         <v>//[WHEN] Assign label to customer card</v>
       </c>
       <c r="K16" s="17" t="str">
-        <f ca="1">[1]!Table29[[#This Row],[ATDD.TestScriptor Format]]</f>
-        <v>When 'Set lookup value on customer card'</v>
+        <f ca="1">IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Assign label to customer card'</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
@@ -1941,8 +1925,8 @@
         <v>//[THEN] Customer has label field populated</v>
       </c>
       <c r="K17" s="17" t="str">
-        <f ca="1">[1]!Table29[[#This Row],[ATDD.TestScriptor Format]]</f>
-        <v>Then 'Customer has lookup value code field populated' } }</v>
+        <f ca="1">IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Customer has label field populated' } }</v>
       </c>
     </row>
     <row r="87" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated Clean ATDD sheet.xlsx
</commit_message>
<xml_diff>
--- a/Excel sheets/Examples/Clean ATDD sheet.xlsx
+++ b/Excel sheets/Examples/Clean ATDD sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvvugt\source\repos\Automated-Testing-in-Microsoft-Dynamics-365-Business-Central-Second-Edition\Excel sheets\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61BA358C-B570-4F9F-B866-EDB5F5D3762F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD96F056-1EDF-4D57-9694-471A08BF7A3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{DB99ADC0-1D36-4CB0-890F-ABAEDD9356F9}"/>
+    <workbookView xWindow="-24690" yWindow="4230" windowWidth="22305" windowHeight="8115" xr2:uid="{DB99ADC0-1D36-4CB0-890F-ABAEDD9356F9}"/>
   </bookViews>
   <sheets>
     <sheet name="ATDD Scenarios" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="46">
   <si>
     <t>Feature</t>
   </si>
@@ -124,15 +124,6 @@
     <t>Assign label to customer card</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>ATDD.TestScriptor Format</t>
   </si>
   <si>
@@ -142,27 +133,6 @@
     <t>FEATURE</t>
   </si>
   <si>
-    <t>SubFeature</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
     <t>A positive-negative scenario</t>
   </si>
   <si>
@@ -170,6 +140,39 @@
   </si>
   <si>
     <t>A scenario</t>
+  </si>
+  <si>
+    <t>MyFeature</t>
+  </si>
+  <si>
+    <t>Do something else</t>
+  </si>
+  <si>
+    <t>Something else happens</t>
+  </si>
+  <si>
+    <t>MySubFeature</t>
+  </si>
+  <si>
+    <t>An error was thrown</t>
+  </si>
+  <si>
+    <t>Something happens</t>
+  </si>
+  <si>
+    <t>Do something</t>
+  </si>
+  <si>
+    <t>Some record</t>
+  </si>
+  <si>
+    <t>Another record</t>
+  </si>
+  <si>
+    <t>Do something in a page</t>
+  </si>
+  <si>
+    <t>Some other Record</t>
   </si>
 </sst>
 </file>
@@ -322,6 +325,9 @@
   </cellStyles>
   <dxfs count="30">
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -340,9 +346,6 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -586,10 +589,10 @@
     <tableColumn id="7" xr3:uid="{762A89F1-1CE0-4623-9ECE-7E18ABCC76DC}" name="Code Format" dataDxfId="2">
       <calculatedColumnFormula>_xlfn.CONCAT("//",Table23[[#This Row],[ATDD Format]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{01376FDB-C35B-4080-A02C-72B0C39BDC01}" name="ATDD.TestScriptor Format" dataDxfId="0">
+    <tableColumn id="11" xr3:uid="{01376FDB-C35B-4080-A02C-72B0C39BDC01}" name="ATDD.TestScriptor Format" dataDxfId="1">
       <calculatedColumnFormula>IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{108458B0-953E-40C3-A10B-F57A3E16C1B8}" name="Notes" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{108458B0-953E-40C3-A10B-F57A3E16C1B8}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -894,9 +897,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08B1ED69-5F96-4A81-993F-0E906F475813}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -904,11 +905,13 @@
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="6" customWidth="1"/>
     <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" style="7" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="32.5703125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="29.85546875" style="7" customWidth="1"/>
+    <col min="10" max="10" width="31" style="7" customWidth="1"/>
+    <col min="11" max="11" width="34.140625" style="7" customWidth="1"/>
     <col min="12" max="12" width="8.5703125" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -923,7 +926,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -944,50 +947,50 @@
         <v>8</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
       <c r="E2" s="19"/>
       <c r="F2" s="11"/>
       <c r="G2" s="21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H2" s="12"/>
       <c r="I2" s="11" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[FEATURE] Feature SubFeature</v>
+        <v>[FEATURE] MyFeature MySubFeature</v>
       </c>
       <c r="J2" s="11" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[FEATURE] Feature SubFeature</v>
+        <v>//[FEATURE] MyFeature MySubFeature</v>
       </c>
       <c r="K2" s="18" t="str">
         <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Feature 'Feature SubFeature' {</v>
+        <v>Feature 'MyFeature MySubFeature' {</v>
       </c>
       <c r="L2" s="11"/>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="H3" s="8">
         <v>1</v>
@@ -1005,105 +1008,105 @@
         <v>Scenario 0001 'A scenario' {</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="H4" s="8">
         <v>1</v>
       </c>
       <c r="I4" s="15" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] A</v>
+        <v>[GIVEN] Some record</v>
       </c>
       <c r="J4" s="16" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] A</v>
+        <v>//[GIVEN] Some record</v>
       </c>
       <c r="K4" s="17" t="str">
         <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'A'</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>Given 'Some record'</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F5" t="s">
         <v>16</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="H5" s="8">
         <v>1</v>
       </c>
       <c r="I5" s="15" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] B</v>
+        <v>[WHEN] Do something</v>
       </c>
       <c r="J5" s="16" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] B</v>
+        <v>//[WHEN] Do something</v>
       </c>
       <c r="K5" s="17" t="str">
         <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'B'</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>When 'Do something'</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F6" t="s">
         <v>18</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="H6" s="8">
         <v>1</v>
       </c>
       <c r="I6" s="15" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] C</v>
+        <v>[THEN] Something happens</v>
       </c>
       <c r="J6" s="16" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] C</v>
+        <v>//[THEN] Something happens</v>
       </c>
       <c r="K6" s="17" t="str">
         <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'C' }</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>Then 'Something happens' }</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>25</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="H7" s="8">
         <v>2</v>
@@ -1121,12 +1124,12 @@
         <v>Scenario 0002 'A positive-negative scenario' {</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>25</v>
@@ -1135,30 +1138,30 @@
         <v>13</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="H8" s="8">
         <v>2</v>
       </c>
       <c r="I8" s="15" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] D</v>
+        <v>[GIVEN] Another record</v>
       </c>
       <c r="J8" s="16" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] D</v>
+        <v>//[GIVEN] Another record</v>
       </c>
       <c r="K8" s="17" t="str">
         <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'D'</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>Given 'Another record'</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>25</v>
@@ -1167,30 +1170,30 @@
         <v>16</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H9" s="8">
         <v>2</v>
       </c>
       <c r="I9" s="15" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] E</v>
+        <v>[WHEN] Do something else</v>
       </c>
       <c r="J9" s="16" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] E</v>
+        <v>//[WHEN] Do something else</v>
       </c>
       <c r="K9" s="17" t="str">
         <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'E'</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>When 'Do something else'</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>25</v>
@@ -1199,36 +1202,36 @@
         <v>18</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H10" s="8">
         <v>2</v>
       </c>
       <c r="I10" s="15" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] F</v>
+        <v>[THEN] An error was thrown</v>
       </c>
       <c r="J10" s="16" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] F</v>
+        <v>//[THEN] An error was thrown</v>
       </c>
       <c r="K10" s="17" t="str">
         <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'F' }</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>Then 'An error was thrown' }</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>25</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="H11" s="8">
         <v>3</v>
@@ -1246,12 +1249,12 @@
         <v>Scenario 0003 'A UI scenario' {</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>25</v>
@@ -1260,30 +1263,30 @@
         <v>13</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="H12" s="8">
         <v>3</v>
       </c>
       <c r="I12" s="15" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] G</v>
+        <v>[GIVEN] Some other Record</v>
       </c>
       <c r="J12" s="16" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] G</v>
+        <v>//[GIVEN] Some other Record</v>
       </c>
       <c r="K12" s="17" t="str">
         <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'G'</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>Given 'Some other Record'</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>25</v>
@@ -1292,30 +1295,30 @@
         <v>16</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H13" s="8">
         <v>3</v>
       </c>
       <c r="I13" s="15" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] H</v>
+        <v>[WHEN] Do something in a page</v>
       </c>
       <c r="J13" s="16" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] H</v>
+        <v>//[WHEN] Do something in a page</v>
       </c>
       <c r="K13" s="17" t="str">
         <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'H'</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>When 'Do something in a page'</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>25</v>
@@ -1324,22 +1327,22 @@
         <v>18</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="H14" s="8">
         <v>3</v>
       </c>
       <c r="I14" s="15" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] I</v>
+        <v>[THEN] Something else happens</v>
       </c>
       <c r="J14" s="16" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] I</v>
+        <v>//[THEN] Something else happens</v>
       </c>
       <c r="K14" s="17" t="str">
         <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'I' } }</v>
+        <v>Then 'Something else happens' } }</v>
       </c>
     </row>
   </sheetData>
@@ -1389,7 +1392,7 @@
   <dimension ref="A1:L108"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1417,7 +1420,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -1438,7 +1441,7 @@
         <v>8</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>9</v>
@@ -1456,7 +1459,7 @@
       <c r="E2" s="19"/>
       <c r="F2" s="9"/>
       <c r="G2" s="21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H2" s="12"/>
       <c r="I2" s="11" t="str">

</xml_diff>

<commit_message>
Updated Clean ATDD Sheet
</commit_message>
<xml_diff>
--- a/Excel sheets/Examples/Clean ATDD sheet.xlsx
+++ b/Excel sheets/Examples/Clean ATDD sheet.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvvugt\source\repos\Automated-Testing-in-Microsoft-Dynamics-365-Business-Central-Second-Edition\Excel sheets\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD96F056-1EDF-4D57-9694-471A08BF7A3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC98498-39D8-4F34-ACE5-E96DC7AAA4DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24690" yWindow="4230" windowWidth="22305" windowHeight="8115" xr2:uid="{DB99ADC0-1D36-4CB0-890F-ABAEDD9356F9}"/>
+    <workbookView xWindow="375" yWindow="4065" windowWidth="21870" windowHeight="8175" xr2:uid="{DB99ADC0-1D36-4CB0-890F-ABAEDD9356F9}"/>
   </bookViews>
   <sheets>
-    <sheet name="ATDD Scenarios" sheetId="1" r:id="rId1"/>
+    <sheet name="ATDD Scenarios" sheetId="3" r:id="rId1"/>
     <sheet name="Examples" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -142,24 +142,12 @@
     <t>A scenario</t>
   </si>
   <si>
-    <t>MyFeature</t>
-  </si>
-  <si>
     <t>Do something else</t>
   </si>
   <si>
-    <t>Something else happens</t>
-  </si>
-  <si>
-    <t>MySubFeature</t>
-  </si>
-  <si>
     <t>An error was thrown</t>
   </si>
   <si>
-    <t>Something happens</t>
-  </si>
-  <si>
     <t>Do something</t>
   </si>
   <si>
@@ -172,7 +160,19 @@
     <t>Do something in a page</t>
   </si>
   <si>
-    <t>Some other Record</t>
+    <t>My Feature</t>
+  </si>
+  <si>
+    <t>My Subfeature</t>
+  </si>
+  <si>
+    <t>Something happened</t>
+  </si>
+  <si>
+    <t>Something else happened</t>
+  </si>
+  <si>
+    <t>Some other record</t>
   </si>
 </sst>
 </file>
@@ -429,6 +429,47 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -442,11 +483,12 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+        <scheme val="none"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -490,47 +532,6 @@
     <dxf>
       <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0070C0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -545,54 +546,54 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D77B0683-CDBE-450E-913A-81EFBBA8B17E}" name="Table2" displayName="Table2" ref="A1:L14" totalsRowShown="0" headerRowDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B61ED27B-D0AA-47A2-AC6F-789FD6DCD64F}" name="Table234" displayName="Table234" ref="A1:L14" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="A1:L14" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{8363E7FF-10AC-4A2B-AF58-2B6F4A3A2982}" name="Feature"/>
-    <tableColumn id="9" xr3:uid="{47ED26B9-CBC1-4AA1-A3A9-843BF13AA89B}" name="Sub Feature"/>
-    <tableColumn id="10" xr3:uid="{2CFDA2E7-B629-4ECF-BE79-854343648AF6}" name="UI" dataDxfId="23"/>
-    <tableColumn id="12" xr3:uid="{42186982-BEE2-4B88-B732-989CDBD8F258}" name="Positive-negative" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{CF058E75-EBE8-492F-899F-08E1336AACB4}" name="Scenario" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{824F4994-529B-42E7-960A-C52362C8177D}" name="Given-When-Then (Tag)"/>
-    <tableColumn id="5" xr3:uid="{9A2C2A27-BDEF-4BD0-8B83-E6DCBCFA35E2}" name="Given-When-Then (Description)" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{357E2CE4-1423-477D-9378-4140E6CC741F}" name="Scenario #" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{A0EF38BD-226F-4389-8485-98738BF5C0B4}" name="ATDD Format" dataDxfId="18">
-      <calculatedColumnFormula>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{58C85A73-07AA-4F26-BFB7-0BB04AFAFB85}" name="Feature"/>
+    <tableColumn id="9" xr3:uid="{CAED13FD-A192-489D-ACC7-AD161E04D5B1}" name="Sub Feature"/>
+    <tableColumn id="10" xr3:uid="{17B98FF8-D93F-486B-94C8-EA4EE070F20C}" name="UI" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{F8AA0F2E-6DFD-4AE9-9803-B6455457F25D}" name="Positive-negative" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{90D467A7-4845-4D0A-9D3B-F8057AF16CE2}" name="Scenario" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{40E32FEA-E95B-4A01-9BF5-606AA95D8581}" name="Given-When-Then (Tag)"/>
+    <tableColumn id="5" xr3:uid="{2016C5DC-D5BE-4D55-BB6D-B506D350D130}" name="Given-When-Then (Description)" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{8BD73CE6-0664-44BF-A4BC-6F2B40AB97D8}" name="Scenario #" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{E8E28F86-AD40-4B27-B599-37D54E069A4E}" name="ATDD Format" dataDxfId="3">
+      <calculatedColumnFormula>IF(Table234[[#This Row],[Given-When-Then (Tag)]]="",IF(Table234[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table234[[#This Row],[Feature]]," ",Table234[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table234[[#This Row],[Scenario '#]],"0000"),"] ",Table234[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table234[[#This Row],[Given-When-Then (Tag)]]),"] ",Table234[[#This Row],[Given-When-Then (Description)]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{55990E10-8959-4AC5-A765-C7364ECDCDE5}" name="Code Format" dataDxfId="17">
-      <calculatedColumnFormula>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</calculatedColumnFormula>
+    <tableColumn id="7" xr3:uid="{33212ECF-9A45-4C9B-93A9-BB95AD894C0B}" name="Code Format" dataDxfId="2">
+      <calculatedColumnFormula>_xlfn.CONCAT("//",Table234[[#This Row],[ATDD Format]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{428C58FA-6B63-4AB1-8578-57C5373BC837}" name="ATDD.TestScriptor Format" dataDxfId="16">
-      <calculatedColumnFormula>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</calculatedColumnFormula>
+    <tableColumn id="11" xr3:uid="{6E96B40C-A7F1-4245-9D95-9464BF370891}" name="ATDD.TestScriptor Format" dataDxfId="1">
+      <calculatedColumnFormula>IF(Table234[[#This Row],[Given-When-Then (Tag)]]="",IF(Table234[[#This Row],[Scenario]]="",IF(Table234[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table234[[#This Row],[Feature]]," ",Table234[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table234[[#This Row],[Scenario '#]],"0000")," '",Table234[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"' } }"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{67272D7F-D0CB-4C6B-967E-B47CC34979CB}" name="Notes" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{0551BD71-6B30-4282-9317-A4450B8EB5FF}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AC94DC61-3A21-44B1-A4FA-D3AE0A291830}" name="Table23" displayName="Table23" ref="A1:L17" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AC94DC61-3A21-44B1-A4FA-D3AE0A291830}" name="Table23" displayName="Table23" ref="A1:L17" totalsRowShown="0" headerRowDxfId="29">
   <autoFilter ref="A1:L17" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{EB12FABE-99EE-4C64-9371-664DA2BC018B}" name="Feature"/>
     <tableColumn id="9" xr3:uid="{C4BF811B-A50B-4F15-ABFB-76F5EF61BAEC}" name="Sub Feature"/>
-    <tableColumn id="10" xr3:uid="{050332A6-04F7-4C80-8BF0-1A37BF66834D}" name="UI" dataDxfId="8"/>
-    <tableColumn id="12" xr3:uid="{91F463C5-D5E2-4E74-89F7-26421CFD4688}" name="Positive-negative" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{F4B03F80-242C-48F3-AD45-4F8870F7CF4C}" name="Scenario" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{050332A6-04F7-4C80-8BF0-1A37BF66834D}" name="UI" dataDxfId="28"/>
+    <tableColumn id="12" xr3:uid="{91F463C5-D5E2-4E74-89F7-26421CFD4688}" name="Positive-negative" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{F4B03F80-242C-48F3-AD45-4F8870F7CF4C}" name="Scenario" dataDxfId="26"/>
     <tableColumn id="3" xr3:uid="{CC6D9ED1-342A-442A-A781-19E1B48EC192}" name="Given-When-Then (Tag)"/>
-    <tableColumn id="5" xr3:uid="{4B77C75B-29B6-4D6D-8295-8BCB00B5A021}" name="Given-When-Then (Description)" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{7A8CEFC7-AFDE-40F5-BF03-D453506926E6}" name="Scenario #" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{4C548BB4-BEA7-4564-81EF-9BD6BCF666EF}" name="ATDD Format" dataDxfId="3">
+    <tableColumn id="5" xr3:uid="{4B77C75B-29B6-4D6D-8295-8BCB00B5A021}" name="Given-When-Then (Description)" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{7A8CEFC7-AFDE-40F5-BF03-D453506926E6}" name="Scenario #" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{4C548BB4-BEA7-4564-81EF-9BD6BCF666EF}" name="ATDD Format" dataDxfId="23">
       <calculatedColumnFormula>IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table23[[#This Row],[Scenario '#]],"0000"),"] ",Table23[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table23[[#This Row],[Given-When-Then (Tag)]]),"] ",Table23[[#This Row],[Given-When-Then (Description)]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{762A89F1-1CE0-4623-9ECE-7E18ABCC76DC}" name="Code Format" dataDxfId="2">
+    <tableColumn id="7" xr3:uid="{762A89F1-1CE0-4623-9ECE-7E18ABCC76DC}" name="Code Format" dataDxfId="22">
       <calculatedColumnFormula>_xlfn.CONCAT("//",Table23[[#This Row],[ATDD Format]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{01376FDB-C35B-4080-A02C-72B0C39BDC01}" name="ATDD.TestScriptor Format" dataDxfId="1">
+    <tableColumn id="11" xr3:uid="{01376FDB-C35B-4080-A02C-72B0C39BDC01}" name="ATDD.TestScriptor Format" dataDxfId="21">
       <calculatedColumnFormula>IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{108458B0-953E-40C3-A10B-F57A3E16C1B8}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{108458B0-953E-40C3-A10B-F57A3E16C1B8}" name="Notes" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -894,25 +895,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08B1ED69-5F96-4A81-993F-0E906F475813}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9C97F81-45CE-49FB-8C99-7D99767A1766}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="6" customWidth="1"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="9" style="5" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="6" customWidth="1"/>
     <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.85546875" style="7" customWidth="1"/>
-    <col min="10" max="10" width="31" style="7" customWidth="1"/>
-    <col min="11" max="11" width="34.140625" style="7" customWidth="1"/>
-    <col min="12" max="12" width="8.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" style="8" customWidth="1"/>
+    <col min="9" max="9" width="26.42578125" style="7" customWidth="1"/>
+    <col min="10" max="10" width="28.5703125" style="7" customWidth="1"/>
+    <col min="11" max="11" width="39" style="7" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -953,41 +956,41 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
       <c r="E2" s="19"/>
-      <c r="F2" s="11"/>
+      <c r="F2" s="9"/>
       <c r="G2" s="21" t="s">
         <v>31</v>
       </c>
       <c r="H2" s="12"/>
       <c r="I2" s="11" t="str">
-        <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[FEATURE] MyFeature MySubFeature</v>
-      </c>
-      <c r="J2" s="11" t="str">
-        <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[FEATURE] MyFeature MySubFeature</v>
+        <f>IF(Table234[[#This Row],[Given-When-Then (Tag)]]="",IF(Table234[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table234[[#This Row],[Feature]]," ",Table234[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table234[[#This Row],[Scenario '#]],"0000"),"] ",Table234[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table234[[#This Row],[Given-When-Then (Tag)]]),"] ",Table234[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[FEATURE] My Feature My Subfeature</v>
+      </c>
+      <c r="J2" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table234[[#This Row],[ATDD Format]])</f>
+        <v>//[FEATURE] My Feature My Subfeature</v>
       </c>
       <c r="K2" s="18" t="str">
-        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Feature 'MyFeature MySubFeature' {</v>
+        <f ca="1">IF(Table234[[#This Row],[Given-When-Then (Tag)]]="",IF(Table234[[#This Row],[Scenario]]="",IF(Table234[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table234[[#This Row],[Feature]]," ",Table234[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table234[[#This Row],[Scenario '#]],"0000")," '",Table234[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Feature 'My Feature My Subfeature' {</v>
       </c>
       <c r="L2" s="11"/>
     </row>
-    <row r="3" spans="1:12" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>34</v>
@@ -995,112 +998,112 @@
       <c r="H3" s="8">
         <v>1</v>
       </c>
-      <c r="I3" s="15" t="str">
-        <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
+      <c r="I3" s="7" t="str">
+        <f>IF(Table234[[#This Row],[Given-When-Then (Tag)]]="",IF(Table234[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table234[[#This Row],[Feature]]," ",Table234[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table234[[#This Row],[Scenario '#]],"0000"),"] ",Table234[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table234[[#This Row],[Given-When-Then (Tag)]]),"] ",Table234[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[SCENARIO #0001] A scenario</v>
       </c>
-      <c r="J3" s="16" t="str">
-        <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
+      <c r="J3" s="14" t="str">
+        <f>_xlfn.CONCAT("//",Table234[[#This Row],[ATDD Format]])</f>
         <v>//[SCENARIO #0001] A scenario</v>
       </c>
       <c r="K3" s="17" t="str">
-        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table234[[#This Row],[Given-When-Then (Tag)]]="",IF(Table234[[#This Row],[Scenario]]="",IF(Table234[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table234[[#This Row],[Feature]]," ",Table234[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table234[[#This Row],[Scenario '#]],"0000")," '",Table234[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0001 'A scenario' {</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H4" s="8">
         <v>1</v>
       </c>
-      <c r="I4" s="15" t="str">
-        <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
+      <c r="I4" s="7" t="str">
+        <f>IF(Table234[[#This Row],[Given-When-Then (Tag)]]="",IF(Table234[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table234[[#This Row],[Feature]]," ",Table234[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table234[[#This Row],[Scenario '#]],"0000"),"] ",Table234[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table234[[#This Row],[Given-When-Then (Tag)]]),"] ",Table234[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[GIVEN] Some record</v>
       </c>
-      <c r="J4" s="16" t="str">
-        <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
+      <c r="J4" s="14" t="str">
+        <f>_xlfn.CONCAT("//",Table234[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Some record</v>
       </c>
       <c r="K4" s="17" t="str">
-        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table234[[#This Row],[Given-When-Then (Tag)]]="",IF(Table234[[#This Row],[Scenario]]="",IF(Table234[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table234[[#This Row],[Feature]]," ",Table234[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table234[[#This Row],[Scenario '#]],"0000")," '",Table234[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Given 'Some record'</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F5" t="s">
         <v>16</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="H5" s="8">
         <v>1</v>
       </c>
-      <c r="I5" s="15" t="str">
-        <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
+      <c r="I5" s="7" t="str">
+        <f>IF(Table234[[#This Row],[Given-When-Then (Tag)]]="",IF(Table234[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table234[[#This Row],[Feature]]," ",Table234[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table234[[#This Row],[Scenario '#]],"0000"),"] ",Table234[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table234[[#This Row],[Given-When-Then (Tag)]]),"] ",Table234[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[WHEN] Do something</v>
       </c>
-      <c r="J5" s="16" t="str">
-        <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
+      <c r="J5" s="14" t="str">
+        <f>_xlfn.CONCAT("//",Table234[[#This Row],[ATDD Format]])</f>
         <v>//[WHEN] Do something</v>
       </c>
       <c r="K5" s="17" t="str">
-        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table234[[#This Row],[Given-When-Then (Tag)]]="",IF(Table234[[#This Row],[Scenario]]="",IF(Table234[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table234[[#This Row],[Feature]]," ",Table234[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table234[[#This Row],[Scenario '#]],"0000")," '",Table234[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>When 'Do something'</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F6" t="s">
         <v>18</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="H6" s="8">
         <v>1</v>
       </c>
-      <c r="I6" s="15" t="str">
-        <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Something happens</v>
-      </c>
-      <c r="J6" s="16" t="str">
-        <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Something happens</v>
+      <c r="I6" s="7" t="str">
+        <f>IF(Table234[[#This Row],[Given-When-Then (Tag)]]="",IF(Table234[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table234[[#This Row],[Feature]]," ",Table234[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table234[[#This Row],[Scenario '#]],"0000"),"] ",Table234[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table234[[#This Row],[Given-When-Then (Tag)]]),"] ",Table234[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Something happened</v>
+      </c>
+      <c r="J6" s="14" t="str">
+        <f>_xlfn.CONCAT("//",Table234[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Something happened</v>
       </c>
       <c r="K6" s="17" t="str">
-        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Something happens' }</v>
+        <f ca="1">IF(Table234[[#This Row],[Given-When-Then (Tag)]]="",IF(Table234[[#This Row],[Scenario]]="",IF(Table234[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table234[[#This Row],[Feature]]," ",Table234[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table234[[#This Row],[Scenario '#]],"0000")," '",Table234[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Something happened' }</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>25</v>
@@ -1111,25 +1114,25 @@
       <c r="H7" s="8">
         <v>2</v>
       </c>
-      <c r="I7" s="15" t="str">
-        <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
+      <c r="I7" s="7" t="str">
+        <f>IF(Table234[[#This Row],[Given-When-Then (Tag)]]="",IF(Table234[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table234[[#This Row],[Feature]]," ",Table234[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table234[[#This Row],[Scenario '#]],"0000"),"] ",Table234[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table234[[#This Row],[Given-When-Then (Tag)]]),"] ",Table234[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[SCENARIO #0002] A positive-negative scenario</v>
       </c>
-      <c r="J7" s="16" t="str">
-        <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
+      <c r="J7" s="14" t="str">
+        <f>_xlfn.CONCAT("//",Table234[[#This Row],[ATDD Format]])</f>
         <v>//[SCENARIO #0002] A positive-negative scenario</v>
       </c>
       <c r="K7" s="17" t="str">
-        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table234[[#This Row],[Given-When-Then (Tag)]]="",IF(Table234[[#This Row],[Scenario]]="",IF(Table234[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table234[[#This Row],[Feature]]," ",Table234[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table234[[#This Row],[Scenario '#]],"0000")," '",Table234[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0002 'A positive-negative scenario' {</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>25</v>
@@ -1138,30 +1141,30 @@
         <v>13</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H8" s="8">
         <v>2</v>
       </c>
       <c r="I8" s="15" t="str">
-        <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
+        <f>IF(Table234[[#This Row],[Given-When-Then (Tag)]]="",IF(Table234[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table234[[#This Row],[Feature]]," ",Table234[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table234[[#This Row],[Scenario '#]],"0000"),"] ",Table234[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table234[[#This Row],[Given-When-Then (Tag)]]),"] ",Table234[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[GIVEN] Another record</v>
       </c>
       <c r="J8" s="16" t="str">
-        <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
+        <f>_xlfn.CONCAT("//",Table234[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Another record</v>
       </c>
       <c r="K8" s="17" t="str">
-        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table234[[#This Row],[Given-When-Then (Tag)]]="",IF(Table234[[#This Row],[Scenario]]="",IF(Table234[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table234[[#This Row],[Feature]]," ",Table234[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table234[[#This Row],[Scenario '#]],"0000")," '",Table234[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Given 'Another record'</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>25</v>
@@ -1170,30 +1173,30 @@
         <v>16</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H9" s="8">
         <v>2</v>
       </c>
       <c r="I9" s="15" t="str">
-        <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
+        <f>IF(Table234[[#This Row],[Given-When-Then (Tag)]]="",IF(Table234[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table234[[#This Row],[Feature]]," ",Table234[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table234[[#This Row],[Scenario '#]],"0000"),"] ",Table234[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table234[[#This Row],[Given-When-Then (Tag)]]),"] ",Table234[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[WHEN] Do something else</v>
       </c>
       <c r="J9" s="16" t="str">
-        <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
+        <f>_xlfn.CONCAT("//",Table234[[#This Row],[ATDD Format]])</f>
         <v>//[WHEN] Do something else</v>
       </c>
       <c r="K9" s="17" t="str">
-        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table234[[#This Row],[Given-When-Then (Tag)]]="",IF(Table234[[#This Row],[Scenario]]="",IF(Table234[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table234[[#This Row],[Feature]]," ",Table234[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table234[[#This Row],[Scenario '#]],"0000")," '",Table234[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>When 'Do something else'</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>25</v>
@@ -1202,30 +1205,30 @@
         <v>18</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H10" s="8">
         <v>2</v>
       </c>
       <c r="I10" s="15" t="str">
-        <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
+        <f>IF(Table234[[#This Row],[Given-When-Then (Tag)]]="",IF(Table234[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table234[[#This Row],[Feature]]," ",Table234[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table234[[#This Row],[Scenario '#]],"0000"),"] ",Table234[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table234[[#This Row],[Given-When-Then (Tag)]]),"] ",Table234[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[THEN] An error was thrown</v>
       </c>
       <c r="J10" s="16" t="str">
-        <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
+        <f>_xlfn.CONCAT("//",Table234[[#This Row],[ATDD Format]])</f>
         <v>//[THEN] An error was thrown</v>
       </c>
       <c r="K10" s="17" t="str">
-        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table234[[#This Row],[Given-When-Then (Tag)]]="",IF(Table234[[#This Row],[Scenario]]="",IF(Table234[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table234[[#This Row],[Feature]]," ",Table234[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table234[[#This Row],[Scenario '#]],"0000")," '",Table234[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Then 'An error was thrown' }</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>25</v>
@@ -1237,24 +1240,24 @@
         <v>3</v>
       </c>
       <c r="I11" s="15" t="str">
-        <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
+        <f>IF(Table234[[#This Row],[Given-When-Then (Tag)]]="",IF(Table234[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table234[[#This Row],[Feature]]," ",Table234[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table234[[#This Row],[Scenario '#]],"0000"),"] ",Table234[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table234[[#This Row],[Given-When-Then (Tag)]]),"] ",Table234[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[SCENARIO #0003] A UI scenario</v>
       </c>
       <c r="J11" s="16" t="str">
-        <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
+        <f>_xlfn.CONCAT("//",Table234[[#This Row],[ATDD Format]])</f>
         <v>//[SCENARIO #0003] A UI scenario</v>
       </c>
       <c r="K11" s="17" t="str">
-        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table234[[#This Row],[Given-When-Then (Tag)]]="",IF(Table234[[#This Row],[Scenario]]="",IF(Table234[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table234[[#This Row],[Feature]]," ",Table234[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table234[[#This Row],[Scenario '#]],"0000")," '",Table234[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0003 'A UI scenario' {</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>25</v>
@@ -1269,24 +1272,24 @@
         <v>3</v>
       </c>
       <c r="I12" s="15" t="str">
-        <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Some other Record</v>
+        <f>IF(Table234[[#This Row],[Given-When-Then (Tag)]]="",IF(Table234[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table234[[#This Row],[Feature]]," ",Table234[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table234[[#This Row],[Scenario '#]],"0000"),"] ",Table234[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table234[[#This Row],[Given-When-Then (Tag)]]),"] ",Table234[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Some other record</v>
       </c>
       <c r="J12" s="16" t="str">
-        <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Some other Record</v>
+        <f>_xlfn.CONCAT("//",Table234[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Some other record</v>
       </c>
       <c r="K12" s="17" t="str">
-        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Some other Record'</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <f ca="1">IF(Table234[[#This Row],[Given-When-Then (Tag)]]="",IF(Table234[[#This Row],[Scenario]]="",IF(Table234[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table234[[#This Row],[Feature]]," ",Table234[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table234[[#This Row],[Scenario '#]],"0000")," '",Table234[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Some other record'</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>25</v>
@@ -1295,30 +1298,30 @@
         <v>16</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H13" s="8">
         <v>3</v>
       </c>
       <c r="I13" s="15" t="str">
-        <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
+        <f>IF(Table234[[#This Row],[Given-When-Then (Tag)]]="",IF(Table234[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table234[[#This Row],[Feature]]," ",Table234[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table234[[#This Row],[Scenario '#]],"0000"),"] ",Table234[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table234[[#This Row],[Given-When-Then (Tag)]]),"] ",Table234[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[WHEN] Do something in a page</v>
       </c>
       <c r="J13" s="16" t="str">
-        <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
+        <f>_xlfn.CONCAT("//",Table234[[#This Row],[ATDD Format]])</f>
         <v>//[WHEN] Do something in a page</v>
       </c>
       <c r="K13" s="17" t="str">
-        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <f ca="1">IF(Table234[[#This Row],[Given-When-Then (Tag)]]="",IF(Table234[[#This Row],[Scenario]]="",IF(Table234[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table234[[#This Row],[Feature]]," ",Table234[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table234[[#This Row],[Scenario '#]],"0000")," '",Table234[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>When 'Do something in a page'</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>25</v>
@@ -1327,32 +1330,32 @@
         <v>18</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="H14" s="8">
         <v>3</v>
       </c>
       <c r="I14" s="15" t="str">
-        <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Something else happens</v>
+        <f>IF(Table234[[#This Row],[Given-When-Then (Tag)]]="",IF(Table234[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table234[[#This Row],[Feature]]," ",Table234[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table234[[#This Row],[Scenario '#]],"0000"),"] ",Table234[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table234[[#This Row],[Given-When-Then (Tag)]]),"] ",Table234[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Something else happened</v>
       </c>
       <c r="J14" s="16" t="str">
-        <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Something else happens</v>
+        <f>_xlfn.CONCAT("//",Table234[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Something else happened</v>
       </c>
       <c r="K14" s="17" t="str">
-        <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Something else happens' } }</v>
+        <f ca="1">IF(Table234[[#This Row],[Given-When-Then (Tag)]]="",IF(Table234[[#This Row],[Scenario]]="",IF(Table234[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table234[[#This Row],[Feature]]," ",Table234[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table234[[#This Row],[Scenario '#]],"0000")," '",Table234[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table234[[#This Row],[Given-When-Then (Tag)]]," '",Table234[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Something else happened' } }</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:D1048576">
-    <cfRule type="cellIs" dxfId="29" priority="13" operator="equal">
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="cellIs" dxfId="19" priority="5" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="colorScale" priority="16">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1364,18 +1367,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1392,7 +1395,7 @@
   <dimension ref="A1:L108"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>